<commit_message>
flower bottle support v3
</commit_message>
<xml_diff>
--- a/flower_support_calcs.xlsx
+++ b/flower_support_calcs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\3D_models\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\local_working\Personal\github\3D_models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ECE3FB0-FE99-45F0-9355-09BE7C58701C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5B449AD-A926-4137-A78A-3CA4CA506D9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="15990" windowWidth="29040" windowHeight="15720" xr2:uid="{C5DFEE08-A576-456A-B64C-E8DF8315E857}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C5DFEE08-A576-456A-B64C-E8DF8315E857}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -482,15 +482,15 @@
   <dimension ref="A1:N31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -498,7 +498,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -510,7 +510,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -522,7 +522,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -530,7 +530,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -538,7 +538,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -551,7 +551,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -559,13 +559,13 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="N11">
         <f>45/2</f>
         <v>22.5</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>5</v>
       </c>
@@ -578,16 +578,20 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>6</v>
+      </c>
+      <c r="B13">
+        <f>C13*2</f>
+        <v>92</v>
       </c>
       <c r="C13">
         <f>C12+B3</f>
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -595,7 +599,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>4</v>
       </c>
@@ -604,7 +608,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -617,15 +621,18 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>10</v>
       </c>
       <c r="B18">
         <v>28</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F18">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -633,7 +640,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -641,7 +648,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -649,7 +656,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -658,7 +665,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -667,7 +674,7 @@
         <v>16.5</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>16</v>
       </c>
@@ -675,7 +682,7 @@
         <v>32.5</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>17</v>
       </c>
@@ -684,7 +691,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>15</v>
       </c>
@@ -692,7 +699,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>18</v>
       </c>
@@ -700,7 +707,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>14</v>
       </c>

</xml_diff>